<commit_message>
[DONE] Unitats amb sub i sup índex des de la taula C7.
Preparació per la taula C1
</commit_message>
<xml_diff>
--- a/public/20220407_SUGGEREIX_Taula_C7.xlsx
+++ b/public/20220407_SUGGEREIX_Taula_C7.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ficra-my.sharepoint.com/personal/mfont_icra_cat/Documents/Documentos/SUGGEREIX_Taules_transformades/Taules_SAD_actuals/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ficra.sharepoint.com/sites/SADSUGGEREIX/Materiales de clase/Doc_SAD_actualitzada/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="11_E3CB737629D1C9335A9414FCAF854A4148002AF9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{338CC687-14A9-4927-A942-53135F529DA2}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="11_E3CB737629D1C9335A9414FCAF854A4148002AF9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{288C0177-ED0E-48A2-8F60-E0D75B5D8120}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="65">
   <si>
     <t>Taula C7. Categories de paràmetres i indicadors: control de la qualitat de l'aigua</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>I1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(pH): unitats de pH </t>
   </si>
   <si>
     <t>I2</t>
@@ -272,12 +269,109 @@
       <t xml:space="preserve">Clostridium perfringens </t>
     </r>
   </si>
+  <si>
+    <t>Unitats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unitats de pH </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pH </t>
+  </si>
+  <si>
+    <t>mg C/l</t>
+  </si>
+  <si>
+    <t>µS/cm</t>
+  </si>
+  <si>
+    <t>NTU</t>
+  </si>
+  <si>
+    <t>mg/l</t>
+  </si>
+  <si>
+    <r>
+      <t>mg/l N-NH</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>mg/l N-NO</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>µ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>g/l</t>
+    </r>
+  </si>
+  <si>
+    <t>CFU/100 ml</t>
+  </si>
+  <si>
+    <t>PFU/100 ml</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -324,6 +418,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -333,7 +439,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -341,11 +447,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -357,6 +472,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,7 +496,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -673,11 +794,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36:C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="34.7109375" style="1" customWidth="1"/>
@@ -685,244 +806,316 @@
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15">
+    <row r="1" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15">
+    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="C3" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="15">
+      <c r="C7" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="P8" s="3"/>
     </row>
-    <row r="9" spans="1:16" ht="15">
+    <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P9" s="3"/>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>12</v>
+      <c r="C10" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="P10" s="3"/>
     </row>
-    <row r="11" spans="1:16" ht="15">
+    <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="P11" s="3"/>
     </row>
-    <row r="12" spans="1:16" ht="15">
+    <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" ht="18.75">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" ht="18.75">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="15">
-      <c r="A16" s="2" t="s">
+    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15">
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="1:2" ht="15">
-      <c r="A20" s="2" t="s">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="1" t="s">
+      <c r="B24" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="1" t="s">
+      <c r="B25" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="C25" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="1" t="s">
+      <c r="B28" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="C28" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
+    </row>
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="5"/>
-    </row>
-    <row r="31" spans="1:2" ht="15">
-      <c r="A31" s="2" t="s">
+    <row r="32" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15">
-      <c r="A35" s="2" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="1" t="s">
+      <c r="B36" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="C36" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="C37" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>53</v>
+      <c r="C38" s="8" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1096,6 +1289,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1104,20 +1303,44 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00851D93-03D9-4DE0-8842-EB56D6423D10}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00851D93-03D9-4DE0-8842-EB56D6423D10}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="758674b2-73ae-44f0-9f19-d4ad379aa2ea"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64C0B8D4-B96B-4DEB-A0B0-AC622BCD6607}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5813D586-A5A5-4F64-8AF7-9E246132DB1A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="758674b2-73ae-44f0-9f19-d4ad379aa2ea"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5813D586-A5A5-4F64-8AF7-9E246132DB1A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64C0B8D4-B96B-4DEB-A0B0-AC622BCD6607}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[DONE] OT3..5, Dummy 1.2 per SAD, bug fix.
</commit_message>
<xml_diff>
--- a/public/20220407_SUGGEREIX_Taula_C7.xlsx
+++ b/public/20220407_SUGGEREIX_Taula_C7.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25301"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ficra.sharepoint.com/sites/SADSUGGEREIX/Materiales de clase/Doc_SAD_actualitzada/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="11_E3CB737629D1C9335A9414FCAF854A4148002AF9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{027603F8-EA73-4021-BAC3-A43EA1776B0E}"/>
+  <xr:revisionPtr revIDLastSave="105" documentId="11_E3CB737629D1C9335A9414FCAF854A4148002AF9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13A420A7-9FC6-4134-8566-6E2127B7F10E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="74">
   <si>
     <t>Taula C7. Categories de paràmetres i indicadors: control de la qualitat de l'aigua</t>
   </si>
@@ -43,51 +43,27 @@
     <t xml:space="preserve">1.1. Paràmetres de monitoratge continu </t>
   </si>
   <si>
-    <t>Unitats</t>
-  </si>
-  <si>
-    <t>Observacions</t>
-  </si>
-  <si>
     <t>I1</t>
   </si>
   <si>
-    <t xml:space="preserve">pH </t>
-  </si>
-  <si>
-    <t xml:space="preserve">unitats de pH </t>
-  </si>
-  <si>
-    <t>Per al pH, no es determinen valors d'eficiència de reducció.</t>
-  </si>
-  <si>
     <t>I2</t>
   </si>
   <si>
     <t>Conductivitat elèctrica</t>
   </si>
   <si>
-    <t>µS/cm</t>
-  </si>
-  <si>
     <t>I3</t>
   </si>
   <si>
     <t>Terbolesa</t>
   </si>
   <si>
-    <t>NTU</t>
-  </si>
-  <si>
     <t>I5</t>
   </si>
   <si>
     <t>Carboni orgànic total (COT)</t>
   </si>
   <si>
-    <t>mg C/l</t>
-  </si>
-  <si>
     <t>1.2 Paràmetres de monitoratge periòdic</t>
   </si>
   <si>
@@ -97,41 +73,10 @@
     <t>Sòlids en suspensió (SST)</t>
   </si>
   <si>
-    <t>mg/l</t>
-  </si>
-  <si>
     <t>2.1. Indicadors químics: nutrients</t>
   </si>
   <si>
     <t>I6</t>
-  </si>
-  <si>
-    <t>Amoni (NH4+)</t>
-  </si>
-  <si>
-    <r>
-      <t>mg/l N-NH</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>+</t>
-    </r>
   </si>
   <si>
     <t>I7</t>
@@ -171,6 +116,166 @@
     </r>
   </si>
   <si>
+    <t>2.2. Indicadors químics: metalls</t>
+  </si>
+  <si>
+    <t>I9</t>
+  </si>
+  <si>
+    <t>Níquel (Ni)</t>
+  </si>
+  <si>
+    <t>I8</t>
+  </si>
+  <si>
+    <t>Zinc (Zn)</t>
+  </si>
+  <si>
+    <t>2.3. Indicadors químics: compostos orgànics</t>
+  </si>
+  <si>
+    <t>I10</t>
+  </si>
+  <si>
+    <t>Carbamazepina</t>
+  </si>
+  <si>
+    <t>I11</t>
+  </si>
+  <si>
+    <t>Diclofenac</t>
+  </si>
+  <si>
+    <t>I15</t>
+  </si>
+  <si>
+    <t>Venlafaxina</t>
+  </si>
+  <si>
+    <t>I16</t>
+  </si>
+  <si>
+    <t>Cafeïna</t>
+  </si>
+  <si>
+    <t>I12</t>
+  </si>
+  <si>
+    <t>N,N-Dietil-m-toluamida (DEET)</t>
+  </si>
+  <si>
+    <t>I13</t>
+  </si>
+  <si>
+    <t>Iopromida</t>
+  </si>
+  <si>
+    <t>I14</t>
+  </si>
+  <si>
+    <t>1,4-Dioxà</t>
+  </si>
+  <si>
+    <t>I17</t>
+  </si>
+  <si>
+    <t>Àcid perfluorooctanosulfònic (PFOS)</t>
+  </si>
+  <si>
+    <t>I18</t>
+  </si>
+  <si>
+    <t>Bis(2-etilhexil) ftalat (DEHP)</t>
+  </si>
+  <si>
+    <t>2.4. Indicadors químics: Productes d'oxidació/transformació</t>
+  </si>
+  <si>
+    <t>Triclorometà</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N-nitrosodimetilamina (NDMA) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Indicadors microbiològics </t>
+  </si>
+  <si>
+    <t>I19</t>
+  </si>
+  <si>
+    <t>Escherichia coli</t>
+  </si>
+  <si>
+    <t>I20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colífags </t>
+  </si>
+  <si>
+    <t>I21</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Espores </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Clostridium perfringens </t>
+    </r>
+  </si>
+  <si>
+    <t>Unitats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unitats de pH </t>
+  </si>
+  <si>
+    <t xml:space="preserve">pH </t>
+  </si>
+  <si>
+    <t>mg C/l</t>
+  </si>
+  <si>
+    <t>µS/cm</t>
+  </si>
+  <si>
+    <t>NTU</t>
+  </si>
+  <si>
+    <t>mg/l</t>
+  </si>
+  <si>
+    <r>
+      <t>mg/l N-NH</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>+</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t>mg/l N-NO</t>
     </r>
@@ -196,15 +301,6 @@
     </r>
   </si>
   <si>
-    <t>2.2. Indicadors químics: metalls</t>
-  </si>
-  <si>
-    <t>I9</t>
-  </si>
-  <si>
-    <t>Níquel (Ni)</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -225,70 +321,16 @@
     </r>
   </si>
   <si>
-    <t>I8</t>
-  </si>
-  <si>
-    <t>Zinc (Zn)</t>
-  </si>
-  <si>
-    <t>2.3. Indicadors químics: compostos orgànics</t>
-  </si>
-  <si>
-    <t>I10</t>
-  </si>
-  <si>
-    <t>Carbamazepina</t>
-  </si>
-  <si>
-    <t>I11</t>
-  </si>
-  <si>
-    <t>Diclofenac</t>
-  </si>
-  <si>
-    <t>I15</t>
-  </si>
-  <si>
-    <t>Venlafaxina</t>
-  </si>
-  <si>
-    <t>I16</t>
-  </si>
-  <si>
-    <t>Cafeïna</t>
-  </si>
-  <si>
-    <t>I12</t>
-  </si>
-  <si>
-    <t>N,N-Dietil-m-toluamida (DEET)</t>
-  </si>
-  <si>
-    <t>I13</t>
-  </si>
-  <si>
-    <t>Iopromida</t>
-  </si>
-  <si>
-    <t>I14</t>
-  </si>
-  <si>
-    <t>1,4-Dioxà</t>
-  </si>
-  <si>
-    <t>I17</t>
-  </si>
-  <si>
-    <t>Àcid perfluorooctanosulfònic (PFOS)</t>
-  </si>
-  <si>
-    <t>I18</t>
-  </si>
-  <si>
-    <t>Bis(2-etilhexil) ftalat (DEHP)</t>
-  </si>
-  <si>
-    <t>2.4. Indicadors químics: Productes d'oxidació/transformació</t>
+    <t>CFU/100 ml</t>
+  </si>
+  <si>
+    <t>PFU/100 ml</t>
+  </si>
+  <si>
+    <t>Per al pH, no es determinen valors d'eficiència de reducció.</t>
+  </si>
+  <si>
+    <t>Observacions</t>
   </si>
   <si>
     <t>Per als indicadors 2.4, el SAD n'indica el risc de formació.</t>
@@ -297,59 +339,35 @@
     <t>OT1</t>
   </si>
   <si>
-    <t>Triclorometà</t>
-  </si>
-  <si>
     <t>OT2</t>
   </si>
   <si>
-    <t xml:space="preserve">N-nitrosodimetilamina (NDMA) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3. Indicadors microbiològics </t>
-  </si>
-  <si>
-    <t>I19</t>
-  </si>
-  <si>
-    <t>Escherichia coli</t>
-  </si>
-  <si>
-    <t>CFU/100 ml</t>
-  </si>
-  <si>
-    <t>I20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Colífags </t>
-  </si>
-  <si>
-    <t>PFU/100 ml</t>
-  </si>
-  <si>
-    <t>I21</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Espores </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Clostridium perfringens </t>
-    </r>
+    <t>Amoni (NH4+)</t>
+  </si>
+  <si>
+    <t>OT3</t>
+  </si>
+  <si>
+    <t>OT4</t>
+  </si>
+  <si>
+    <t>OT5</t>
+  </si>
+  <si>
+    <t>Clorat</t>
+  </si>
+  <si>
+    <t>Clorit</t>
+  </si>
+  <si>
+    <t>Bromat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -408,6 +426,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -429,7 +454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -442,6 +467,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -462,7 +494,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -758,13 +790,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P38"/>
+  <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="34.7109375" style="1" customWidth="1"/>
@@ -772,325 +804,355 @@
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15">
+    <row r="1" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15">
+    <row r="3" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="15">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="P8" s="3"/>
     </row>
-    <row r="9" spans="1:16" ht="15">
+    <row r="9" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="P9" s="3"/>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="P10" s="3"/>
     </row>
-    <row r="11" spans="1:16" ht="15">
+    <row r="11" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="P11" s="3"/>
     </row>
-    <row r="12" spans="1:16" ht="15">
+    <row r="12" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="18.75">
-      <c r="A13" s="1" t="s">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C21" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" ht="18.75">
-      <c r="A14" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C22" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" ht="15">
-      <c r="A16" s="2" t="s">
+      <c r="C26" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="15">
-      <c r="A17" s="1" t="s">
+      <c r="B27" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15">
-      <c r="A18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15">
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" ht="15">
-      <c r="A20" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15">
-      <c r="A21" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="1" t="s">
+      <c r="C27" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15">
-      <c r="A22" s="1" t="s">
+      <c r="B28" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C28" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15">
-      <c r="A23" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C29" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="5"/>
+    </row>
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15">
-      <c r="A24" s="1" t="s">
+      <c r="D31" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="C32" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15">
-      <c r="A25" s="1" t="s">
+      <c r="C33" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="3" t="s">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15">
-      <c r="A26" s="1" t="s">
+      <c r="B39" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C39" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="15">
-      <c r="A27" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C40" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15">
-      <c r="A28" s="1" t="s">
+      <c r="B41" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15">
-      <c r="A29" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="5"/>
-    </row>
-    <row r="31" spans="1:4" ht="15">
-      <c r="A31" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15">
-      <c r="A32" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15">
-      <c r="A33" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15">
-      <c r="A35" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="1" t="s">
+      <c r="C41" s="9" t="s">
         <v>60</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1100,12 +1162,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010042169B78D842A848BE799D251A5B2C6A" ma:contentTypeVersion="7" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="625099e38fc716cc4bb30b36cfa7c837">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="758674b2-73ae-44f0-9f19-d4ad379aa2ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c97fa59194b5c482d1d5e2dd6e3e6b4b" ns2:_="">
     <xsd:import namespace="758674b2-73ae-44f0-9f19-d4ad379aa2ea"/>
@@ -1269,7 +1325,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1278,14 +1334,50 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5813D586-A5A5-4F64-8AF7-9E246132DB1A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00851D93-03D9-4DE0-8842-EB56D6423D10}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="758674b2-73ae-44f0-9f19-d4ad379aa2ea"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00851D93-03D9-4DE0-8842-EB56D6423D10}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64C0B8D4-B96B-4DEB-A0B0-AC622BCD6607}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64C0B8D4-B96B-4DEB-A0B0-AC622BCD6607}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5813D586-A5A5-4F64-8AF7-9E246132DB1A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="758674b2-73ae-44f0-9f19-d4ad379aa2ea"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>